<commit_message>
added gene model info scatter plot. redownloaded bash scripts for creating the fiveSpecies
</commit_message>
<xml_diff>
--- a/bankole_sex_specific_splicing_2024/documentation/create_fiveSpecies_annotation_per_genome_13ksb.xlsx
+++ b/bankole_sex_specific_splicing_2024/documentation/create_fiveSpecies_annotation_per_genome_13ksb.xlsx
@@ -69,6 +69,7 @@
         <sz val="11"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/blue/mcintyre/k.bankole/github/TranD/utilities</t>
     </r>
@@ -735,21 +736,21 @@
   </si>
   <si>
     <t xml:space="preserve">PROJ/mapped_ujc_id_ujc_output/
-dyak21_2_dyak2_ujc_2_dmel6_noGeneID_ujc_dscrptn.csv
-dsimWXD_2_dsim2_ujc_2_dmel6_noGeneID_ujc_dscrptn.csv
+dyak21_2_dyak2_ujc_2_dmel6_noGeneID_ujc_info.csv
+dsimWXD_2_dsim2_ujc_2_dmel6_noGeneID_ujc_info.csv
 dsan11_2_dsan1_ujc_2_dmel6_noGeneID_ujc.gtf
 dsim202_2_dsim2_ujc_2_dmel6_noGeneID_ujc.gtf
-dser11_2_dser1_ujc_2_dmel6_noGeneID_ujc_dscrptn.csv
+dser11_2_dser1_ujc_2_dmel6_noGeneID_ujc_info.csv
 dsimWXD_2_dsim2_ujc_2_dmel6_noGeneID_ujc_xscript_link.csv
 dsimWXD_2_dsim2_ujc_2_dmel6_noGeneID_ujc.gtf
 dyak21_2_dyak2_ujc_2_dmel6_noGeneID_ujc.gtf
 dser11_2_dser1_ujc_2_dmel6_noGeneID_ujc.gtf
 dser11_2_dser1_ujc_2_dmel6_noGeneID_ujc_xscript_link.csv
-dsan11_2_dsan1_ujc_2_dmel6_noGeneID_ujc_dscrptn.csv
+dsan11_2_dsan1_ujc_2_dmel6_noGeneID_ujc_info.csv
 dyak21_2_dyak2_ujc_2_dmel6_noGeneID_ujc_xscript_link.csv
 dsim202_2_dsim2_ujc_2_dmel6_noGeneID_ujc_xscript_link.csv
 dsan11_2_dsan1_ujc_2_dmel6_noGeneID_ujc_xscript_link.csv
-dsim202_2_dsim2_ujc_2_dmel6_noGeneID_ujc_dscrptn.csv</t>
+dsim202_2_dsim2_ujc_2_dmel6_noGeneID_ujc_info.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Count number of UJCs:
@@ -815,16 +816,16 @@
     <t xml:space="preserve">PROJ/mapped_ujc_id_ujc_output/
 dyak21_2_dyak2_ujc_2_dsim2_noGeneID_ujc_xscript_link.csv
 dsan11_2_dsan1_ujc_2_dsim2_noGeneID_ujc.gtf
-dser11_2_dser1_ujc_2_dsim2_noGeneID_ujc_dscrptn.csv
+dser11_2_dser1_ujc_2_dsim2_noGeneID_ujc_info.csv
 dser11_2_dser1_ujc_2_dsim2_noGeneID_ujc.gtf
 dyak21_2_dyak2_ujc_2_dsim2_noGeneID_ujc.gtf
 dmel650_2_dmel6_ujc_2_dsim2_noGeneID_ujc.gtf
-dmel650_2_dmel6_ujc_2_dsim2_noGeneID_ujc_dscrptn.csv
-dsan11_2_dsan1_ujc_2_dsim2_noGeneID_ujc_dscrptn.csv
+dmel650_2_dmel6_ujc_2_dsim2_noGeneID_ujc_info.csv
+dsan11_2_dsan1_ujc_2_dsim2_noGeneID_ujc_info.csv
 dser11_2_dser1_ujc_2_dsim2_noGeneID_ujc_xscript_link.csv
 dmel650_2_dmel6_ujc_2_dsim2_noGeneID_ujc_xscript_link.csv
 dsan11_2_dsan1_ujc_2_dsim2_noGeneID_ujc_xscript_link.csv
-dyak21_2_dyak2_ujc_2_dsim2_noGeneID_ujc_dscrptn.csv
+dyak21_2_dyak2_ujc_2_dsim2_noGeneID_ujc_info.csv
 </t>
   </si>
   <si>
@@ -886,21 +887,21 @@
   </si>
   <si>
     <t xml:space="preserve">PROJ/mapped_ujc_id_ujc_output/
-dser11_2_dser1_ujc_2_dsan1_noGeneID_ujc_dscrptn.csv
+dser11_2_dser1_ujc_2_dsan1_noGeneID_ujc_info.csv
 dmel650_2_dmel6_ujc_2_dsan1_noGeneID_ujc.gtf
-dsim202_2_dsim2_ujc_2_dsan1_noGeneID_ujc_dscrptn.csv
+dsim202_2_dsim2_ujc_2_dsan1_noGeneID_ujc_info.csv
 dser11_2_dser1_ujc_2_dsan1_noGeneID_ujc_xscript_link.csv
 dmel650_2_dmel6_ujc_2_dsan1_noGeneID_ujc_xscript_link.csv
 dsim202_2_dsim2_ujc_2_dsan1_noGeneID_ujc_xscript_link.csv
 dser11_2_dser1_ujc_2_dsan1_noGeneID_ujc.gtf
-dsimWXD_2_dsim2_ujc_2_dsan1_noGeneID_ujc_dscrptn.csv
+dsimWXD_2_dsim2_ujc_2_dsan1_noGeneID_ujc_info.csv
 dyak21_2_dyak2_ujc_2_dsan1_noGeneID_ujc_xscript_link.csv
 dyak21_2_dyak2_ujc_2_dsan1_noGeneID_ujc.gtf
-dyak21_2_dyak2_ujc_2_dsan1_noGeneID_ujc_dscrptn.csv
+dyak21_2_dyak2_ujc_2_dsan1_noGeneID_ujc_info.csv
 dsimWXD_2_dsim2_ujc_2_dsan1_noGeneID_ujc_xscript_link.csv
 dsimWXD_2_dsim2_ujc_2_dsan1_noGeneID_ujc.gtf
 dsim202_2_dsim2_ujc_2_dsan1_noGeneID_ujc.gtf
-dmel650_2_dmel6_ujc_2_dsan1_noGeneID_ujc_dscrptn.csv</t>
+dmel650_2_dmel6_ujc_2_dsan1_noGeneID_ujc_info.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Count number of UJCs:
@@ -964,16 +965,16 @@
   <si>
     <t xml:space="preserve">PROJ/mapped_ujc_id_ujc_output/
 dser11_2_dser1_ujc_2_dyak2_noGeneID_ujc.gtf
-dsan11_2_dsan1_ujc_2_dyak2_noGeneID_ujc_dscrptn.csv
-dsimWXD_2_dsim2_ujc_2_dyak2_noGeneID_ujc_dscrptn.csv
+dsan11_2_dsan1_ujc_2_dyak2_noGeneID_ujc_info.csv
+dsimWXD_2_dsim2_ujc_2_dyak2_noGeneID_ujc_info.csv
 dsim202_2_dsim2_ujc_2_dyak2_noGeneID_ujc_xscript_link.csv
-dmel650_2_dmel6_ujc_2_dyak2_noGeneID_ujc_dscrptn.csv
+dmel650_2_dmel6_ujc_2_dyak2_noGeneID_ujc_info.csv
 dsimWXD_2_dsim2_ujc_2_dyak2_noGeneID_ujc.gtf
 dsimWXD_2_dsim2_ujc_2_dyak2_noGeneID_ujc_xscript_link.csv
 dsim202_2_dsim2_ujc_2_dyak2_noGeneID_ujc.gtf
 dmel650_2_dmel6_ujc_2_dyak2_noGeneID_ujc.gtf
-dser11_2_dser1_ujc_2_dyak2_noGeneID_ujc_dscrptn.csv
-dsim202_2_dsim2_ujc_2_dyak2_noGeneID_ujc_dscrptn.csv
+dser11_2_dser1_ujc_2_dyak2_noGeneID_ujc_info.csv
+dsim202_2_dsim2_ujc_2_dyak2_noGeneID_ujc_info.csv
 dsan11_2_dsan1_ujc_2_dyak2_noGeneID_ujc.gtf
 dmel650_2_dmel6_ujc_2_dyak2_noGeneID_ujc_xscript_link.csv
 dser11_2_dser1_ujc_2_dyak2_noGeneID_ujc_xscript_link.csv
@@ -1045,17 +1046,17 @@
     <t xml:space="preserve">PROJ/mapped_ujc_id_ujc_output/
 dsim202_2_dsim2_ujc_2_dser1_noGeneID_ujc_xscript_link.csv
 dsimWXD_2_dsim2_ujc_2_dser1_noGeneID_ujc.gtf
-dsim202_2_dsim2_ujc_2_dser1_noGeneID_ujc_dscrptn.csv
+dsim202_2_dsim2_ujc_2_dser1_noGeneID_ujc_info.csv
 dsan11_2_dsan1_ujc_2_dser1_noGeneID_ujc.gtf
 dyak21_2_dyak2_ujc_2_dser1_noGeneID_ujc.gtf
 dyak21_2_dyak2_ujc_2_dser1_noGeneID_ujc_xscript_link.csv
-dsan11_2_dsan1_ujc_2_dser1_noGeneID_ujc_dscrptn.csv
+dsan11_2_dsan1_ujc_2_dser1_noGeneID_ujc_info.csv
 dsim202_2_dsim2_ujc_2_dser1_noGeneID_ujc.gtf
 dsimWXD_2_dsim2_ujc_2_dser1_noGeneID_ujc_xscript_link.csv
-dsimWXD_2_dsim2_ujc_2_dser1_noGeneID_ujc_dscrptn.csv
-dyak21_2_dyak2_ujc_2_dser1_noGeneID_ujc_dscrptn.csv
+dsimWXD_2_dsim2_ujc_2_dser1_noGeneID_ujc_info.csv
+dyak21_2_dyak2_ujc_2_dser1_noGeneID_ujc_info.csv
 dmel650_2_dmel6_ujc_2_dser1_noGeneID_ujc.gtf
-dmel650_2_dmel6_ujc_2_dser1_noGeneID_ujc_dscrptn.csv
+dmel650_2_dmel6_ujc_2_dser1_noGeneID_ujc_info.csv
 dmel650_2_dmel6_ujc_2_dser1_noGeneID_ujc_xscript_link.csv
 dsan11_2_dsan1_ujc_2_dser1_noGeneID_ujc_xscript_link.csv
 </t>
@@ -1646,6 +1647,7 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1968,8 +1970,8 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C52" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C66" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H67" activeCellId="0" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9921875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2636,7 +2638,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="282.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="283.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>